<commit_message>
Time-series Graph Updated to include figures
</commit_message>
<xml_diff>
--- a/TimeSeries Data.xlsx
+++ b/TimeSeries Data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dzobo/Desktop/kalyppo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewabb/Dropbox/Ashesi/Data Mining/KalyppoChallenge/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="20460"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16900"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,9 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
   </pivotCaches>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -4786,7 +4783,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4905,6 +4902,64 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$I$3:$I$38</c:f>
@@ -5142,7 +5197,7 @@
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -5150,11 +5205,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2123444448"/>
-        <c:axId val="-2099901792"/>
+        <c:axId val="-2084889712"/>
+        <c:axId val="-2079160416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2123444448"/>
+        <c:axId val="-2084889712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5197,7 +5252,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2099901792"/>
+        <c:crossAx val="-2079160416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5205,57 +5260,17 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2099901792"/>
+        <c:axId val="-2079160416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-2123444448"/>
+        <c:crossAx val="-2084889712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5267,6 +5282,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -5852,13 +5899,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>650240</xdr:colOff>
+      <xdr:colOff>650239</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>182880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>200525</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
@@ -12760,7 +12807,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="F2:G40" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -13239,17 +13286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2272"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:G3"/>
-      <pivotSelection pane="bottomRight" showHeader="1" extendable="1" axis="axisRow" max="38" activeRow="2" activeCol="5" previousRow="2" previousCol="5" click="1" r:id="rId1">
-        <pivotArea dataOnly="0" axis="axisRow" fieldPosition="0">
-          <references count="1">
-            <reference field="0" count="1">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotSelection>
+    <sheetView tabSelected="1" zoomScale="57" workbookViewId="0">
+      <selection activeCell="AJ11" sqref="AJ11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>